<commit_message>
import_scan add kanban nr
</commit_message>
<xml_diff>
--- a/pms-server/uploadfiles/template/kanban_scan.xlsx
+++ b/pms-server/uploadfiles/template/kanban_scan.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25703"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25808"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liqi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liqi/projects/work/pms/pms-server/uploadfiles/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Wire Nr</t>
   </si>
   <si>
     <t>Product Nr</t>
+  </si>
+  <si>
+    <t>Kanban Nr</t>
   </si>
 </sst>
 </file>
@@ -344,19 +347,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>